<commit_message>
Fix duplicate on hayday ingredients
</commit_message>
<xml_diff>
--- a/Excel/hayday.xlsx
+++ b/Excel/hayday.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Asset Factory\HayDay Products\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\All Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C9FFA7-300F-439B-8691-3589F02CA50B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93712DD5-B5CD-45CE-9CAC-60BBE1D98759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11088" yWindow="228" windowWidth="11940" windowHeight="6192" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10296" yWindow="372" windowWidth="12744" windowHeight="6192" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goods" sheetId="1" r:id="rId1"/>
@@ -3069,8 +3069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K356"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B351" sqref="B351"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B127" sqref="B127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13454,8 +13454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3414857B-17AF-4107-83E0-9CC76FB79584}">
   <dimension ref="A1:F725"/>
   <sheetViews>
-    <sheetView topLeftCell="A706" workbookViewId="0">
-      <selection activeCell="E726" sqref="E726"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="D183" sqref="D183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14141,7 +14141,7 @@
         <v>116</v>
       </c>
       <c r="B59">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -15538,7 +15538,7 @@
         <v>169</v>
       </c>
       <c r="B186">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C186">
         <v>1</v>

</xml_diff>

<commit_message>
Fix hayday goods typo
</commit_message>
<xml_diff>
--- a/Excel/hayday.xlsx
+++ b/Excel/hayday.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\All Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93712DD5-B5CD-45CE-9CAC-60BBE1D98759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29732905-776C-4824-A7CF-2BD1312B576B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10296" yWindow="372" windowWidth="12744" windowHeight="6192" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goods" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,10 @@
     <sheet name="Producers" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_data.xlsxBuildingsTable1" hidden="1">BuildingsTable[]</definedName>
-    <definedName name="_xlcn.WorksheetConnection_data.xlsxGoodsTable1" hidden="1">GoodsTable[]</definedName>
-    <definedName name="_xlcn.WorksheetConnection_data.xlsxIngredientsTable1" hidden="1">IngredientsTable[]</definedName>
-    <definedName name="_xlcn.WorksheetConnection_data.xlsxProducersTable1" hidden="1">ProducersTable[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_data.xlsxBuildingsTable" hidden="1">BuildingsTable[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_data.xlsxGoodsTable" hidden="1">GoodsTable[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_data.xlsxIngredientsTable" hidden="1">IngredientsTable[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_data.xlsxProducersTable" hidden="1">ProducersTable[]</definedName>
     <definedName name="Goods">Goods!$A$1:$H$356</definedName>
     <definedName name="Ingredients">Ingredients!$A$1:$C$466</definedName>
   </definedNames>
@@ -73,7 +73,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="BuildingsTable">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_data.xlsxBuildingsTable1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_data.xlsxBuildingsTable"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -82,7 +82,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="GoodsTable">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_data.xlsxGoodsTable1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_data.xlsxGoodsTable"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -91,7 +91,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="IngredientsTable">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_data.xlsxIngredientsTable1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_data.xlsxIngredientsTable"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -100,7 +100,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="ProducersTable">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_data.xlsxProducersTable1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_data.xlsxProducersTable"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -1197,9 +1197,6 @@
     <t>Wooly Chaps</t>
   </si>
   <si>
-    <t>wolly_chaps</t>
-  </si>
-  <si>
     <t>Cream Cake</t>
   </si>
   <si>
@@ -1359,9 +1356,6 @@
     <t>Wheat Bundle</t>
   </si>
   <si>
-    <t>wheat_bundles</t>
-  </si>
-  <si>
     <t>Strawberry Cake</t>
   </si>
   <si>
@@ -1434,12 +1428,6 @@
     <t>potato_bread</t>
   </si>
   <si>
-    <t>Shepheard's Pie</t>
-  </si>
-  <si>
-    <t>shepheards_pie</t>
-  </si>
-  <si>
     <t>Chocolate Ice Cream</t>
   </si>
   <si>
@@ -2593,6 +2581,18 @@
   </si>
   <si>
     <t>rice_ball</t>
+  </si>
+  <si>
+    <t>wooly_chaps</t>
+  </si>
+  <si>
+    <t>wheat_bundle</t>
+  </si>
+  <si>
+    <t>Shepherd's Pie</t>
+  </si>
+  <si>
+    <t>shepherds_pie</t>
   </si>
 </sst>
 </file>
@@ -3069,8 +3069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K356"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B127" sqref="B127"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="C154" sqref="C154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3107,7 +3107,7 @@
         <v>54</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -6456,7 +6456,7 @@
         <v>361</v>
       </c>
       <c r="C115" t="s">
-        <v>362</v>
+        <v>824</v>
       </c>
       <c r="D115" t="s">
         <v>314</v>
@@ -6482,10 +6482,10 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
+        <v>362</v>
+      </c>
+      <c r="C116" t="s">
         <v>363</v>
-      </c>
-      <c r="C116" t="s">
-        <v>364</v>
       </c>
       <c r="D116" t="s">
         <v>314</v>
@@ -6512,10 +6512,10 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
+        <v>364</v>
+      </c>
+      <c r="C117" t="s">
         <v>365</v>
-      </c>
-      <c r="C117" t="s">
-        <v>366</v>
       </c>
       <c r="D117" t="s">
         <v>314</v>
@@ -6541,10 +6541,10 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
+        <v>366</v>
+      </c>
+      <c r="C118" t="s">
         <v>367</v>
-      </c>
-      <c r="C118" t="s">
-        <v>368</v>
       </c>
       <c r="D118" t="s">
         <v>314</v>
@@ -6571,10 +6571,10 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
+        <v>368</v>
+      </c>
+      <c r="C119" t="s">
         <v>369</v>
-      </c>
-      <c r="C119" t="s">
-        <v>370</v>
       </c>
       <c r="D119" t="s">
         <v>314</v>
@@ -6601,10 +6601,10 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
+        <v>370</v>
+      </c>
+      <c r="C120" t="s">
         <v>371</v>
-      </c>
-      <c r="C120" t="s">
-        <v>372</v>
       </c>
       <c r="D120" t="s">
         <v>314</v>
@@ -6630,10 +6630,10 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
+        <v>372</v>
+      </c>
+      <c r="C121" t="s">
         <v>373</v>
-      </c>
-      <c r="C121" t="s">
-        <v>374</v>
       </c>
       <c r="D121" t="s">
         <v>314</v>
@@ -6660,10 +6660,10 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
+        <v>374</v>
+      </c>
+      <c r="C122" t="s">
         <v>375</v>
-      </c>
-      <c r="C122" t="s">
-        <v>376</v>
       </c>
       <c r="D122" t="s">
         <v>314</v>
@@ -6690,10 +6690,10 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
+        <v>376</v>
+      </c>
+      <c r="C123" t="s">
         <v>377</v>
-      </c>
-      <c r="C123" t="s">
-        <v>378</v>
       </c>
       <c r="D123" t="s">
         <v>314</v>
@@ -6720,10 +6720,10 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
+        <v>378</v>
+      </c>
+      <c r="C124" t="s">
         <v>379</v>
-      </c>
-      <c r="C124" t="s">
-        <v>380</v>
       </c>
       <c r="D124" t="s">
         <v>314</v>
@@ -6750,10 +6750,10 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
+        <v>380</v>
+      </c>
+      <c r="C125" t="s">
         <v>381</v>
-      </c>
-      <c r="C125" t="s">
-        <v>382</v>
       </c>
       <c r="D125" t="s">
         <v>314</v>
@@ -6779,10 +6779,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
+        <v>382</v>
+      </c>
+      <c r="C126" t="s">
         <v>383</v>
-      </c>
-      <c r="C126" t="s">
-        <v>384</v>
       </c>
       <c r="D126" t="s">
         <v>314</v>
@@ -6808,10 +6808,10 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
+        <v>384</v>
+      </c>
+      <c r="C127" t="s">
         <v>385</v>
-      </c>
-      <c r="C127" t="s">
-        <v>386</v>
       </c>
       <c r="D127" t="s">
         <v>314</v>
@@ -6838,10 +6838,10 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
+        <v>386</v>
+      </c>
+      <c r="C128" t="s">
         <v>387</v>
-      </c>
-      <c r="C128" t="s">
-        <v>388</v>
       </c>
       <c r="D128" t="s">
         <v>314</v>
@@ -6867,10 +6867,10 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
+        <v>388</v>
+      </c>
+      <c r="C129" t="s">
         <v>389</v>
-      </c>
-      <c r="C129" t="s">
-        <v>390</v>
       </c>
       <c r="D129" t="s">
         <v>314</v>
@@ -6896,10 +6896,10 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
+        <v>390</v>
+      </c>
+      <c r="C130" t="s">
         <v>391</v>
-      </c>
-      <c r="C130" t="s">
-        <v>392</v>
       </c>
       <c r="D130" t="s">
         <v>314</v>
@@ -6925,10 +6925,10 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
+        <v>392</v>
+      </c>
+      <c r="C131" t="s">
         <v>393</v>
-      </c>
-      <c r="C131" t="s">
-        <v>394</v>
       </c>
       <c r="D131" t="s">
         <v>314</v>
@@ -6955,10 +6955,10 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
+        <v>394</v>
+      </c>
+      <c r="C132" t="s">
         <v>395</v>
-      </c>
-      <c r="C132" t="s">
-        <v>396</v>
       </c>
       <c r="D132" t="s">
         <v>314</v>
@@ -6984,10 +6984,10 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
+        <v>396</v>
+      </c>
+      <c r="C133" t="s">
         <v>397</v>
-      </c>
-      <c r="C133" t="s">
-        <v>398</v>
       </c>
       <c r="D133" t="s">
         <v>314</v>
@@ -7013,10 +7013,10 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
+        <v>398</v>
+      </c>
+      <c r="C134" t="s">
         <v>399</v>
-      </c>
-      <c r="C134" t="s">
-        <v>400</v>
       </c>
       <c r="D134" t="s">
         <v>314</v>
@@ -7043,10 +7043,10 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
+        <v>400</v>
+      </c>
+      <c r="C135" t="s">
         <v>401</v>
-      </c>
-      <c r="C135" t="s">
-        <v>402</v>
       </c>
       <c r="D135" t="s">
         <v>314</v>
@@ -7073,10 +7073,10 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
+        <v>402</v>
+      </c>
+      <c r="C136" t="s">
         <v>403</v>
-      </c>
-      <c r="C136" t="s">
-        <v>404</v>
       </c>
       <c r="D136" t="s">
         <v>314</v>
@@ -7102,10 +7102,10 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
+        <v>404</v>
+      </c>
+      <c r="C137" t="s">
         <v>405</v>
-      </c>
-      <c r="C137" t="s">
-        <v>406</v>
       </c>
       <c r="D137" t="s">
         <v>314</v>
@@ -7132,10 +7132,10 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
+        <v>406</v>
+      </c>
+      <c r="C138" t="s">
         <v>407</v>
-      </c>
-      <c r="C138" t="s">
-        <v>408</v>
       </c>
       <c r="D138" t="s">
         <v>314</v>
@@ -7162,10 +7162,10 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="C139" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="D139" t="s">
         <v>314</v>
@@ -7192,10 +7192,10 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
+        <v>408</v>
+      </c>
+      <c r="C140" t="s">
         <v>409</v>
-      </c>
-      <c r="C140" t="s">
-        <v>410</v>
       </c>
       <c r="D140" t="s">
         <v>314</v>
@@ -7222,10 +7222,10 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
+        <v>410</v>
+      </c>
+      <c r="C141" t="s">
         <v>411</v>
-      </c>
-      <c r="C141" t="s">
-        <v>412</v>
       </c>
       <c r="D141" t="s">
         <v>314</v>
@@ -7252,10 +7252,10 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
+        <v>412</v>
+      </c>
+      <c r="C142" t="s">
         <v>413</v>
-      </c>
-      <c r="C142" t="s">
-        <v>414</v>
       </c>
       <c r="D142" t="s">
         <v>314</v>
@@ -7282,10 +7282,10 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C143" t="s">
-        <v>416</v>
+        <v>825</v>
       </c>
       <c r="D143" t="s">
         <v>314</v>
@@ -7312,10 +7312,10 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C144" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D144" t="s">
         <v>314</v>
@@ -7342,10 +7342,10 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C145" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D145" t="s">
         <v>314</v>
@@ -7372,10 +7372,10 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C146" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D146" t="s">
         <v>314</v>
@@ -7402,10 +7402,10 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C147" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D147" t="s">
         <v>314</v>
@@ -7431,10 +7431,10 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C148" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D148" t="s">
         <v>314</v>
@@ -7461,10 +7461,10 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C149" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D149" t="s">
         <v>314</v>
@@ -7491,10 +7491,10 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C150" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D150" t="s">
         <v>314</v>
@@ -7521,10 +7521,10 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C151" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D151" t="s">
         <v>314</v>
@@ -7551,10 +7551,10 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C152" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D152" t="s">
         <v>314</v>
@@ -7580,10 +7580,10 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C153" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D153" t="s">
         <v>314</v>
@@ -7610,10 +7610,10 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C154" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D154" t="s">
         <v>314</v>
@@ -7640,10 +7640,10 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C155" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D155" t="s">
         <v>314</v>
@@ -7670,10 +7670,10 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>441</v>
+        <v>826</v>
       </c>
       <c r="C156" t="s">
-        <v>442</v>
+        <v>827</v>
       </c>
       <c r="D156" t="s">
         <v>314</v>
@@ -7700,10 +7700,10 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="C157" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="D157" t="s">
         <v>314</v>
@@ -7730,10 +7730,10 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="C158" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="D158" t="s">
         <v>314</v>
@@ -7759,10 +7759,10 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C159" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="D159" t="s">
         <v>314</v>
@@ -7788,10 +7788,10 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="C160" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="D160" t="s">
         <v>314</v>
@@ -7818,10 +7818,10 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C161" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D161" t="s">
         <v>314</v>
@@ -7848,10 +7848,10 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="C162" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="D162" t="s">
         <v>314</v>
@@ -7878,10 +7878,10 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C163" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="D163" t="s">
         <v>314</v>
@@ -7907,10 +7907,10 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C164" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="D164" t="s">
         <v>314</v>
@@ -7936,10 +7936,10 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="C165" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="D165" t="s">
         <v>314</v>
@@ -7966,10 +7966,10 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="C166" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="D166" t="s">
         <v>314</v>
@@ -7995,10 +7995,10 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C167" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D167" t="s">
         <v>314</v>
@@ -8025,10 +8025,10 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="C168" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="D168" t="s">
         <v>314</v>
@@ -8055,10 +8055,10 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C169" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D169" t="s">
         <v>314</v>
@@ -8084,10 +8084,10 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C170" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="D170" t="s">
         <v>314</v>
@@ -8114,10 +8114,10 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C171" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D171" t="s">
         <v>314</v>
@@ -8144,10 +8144,10 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C172" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="D172" t="s">
         <v>314</v>
@@ -8174,10 +8174,10 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="C173" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="D173" t="s">
         <v>314</v>
@@ -8204,10 +8204,10 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="C174" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="D174" t="s">
         <v>314</v>
@@ -8234,10 +8234,10 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C175" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D175" t="s">
         <v>314</v>
@@ -8264,10 +8264,10 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="C176" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="D176" t="s">
         <v>314</v>
@@ -8294,10 +8294,10 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C177" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="D177" t="s">
         <v>314</v>
@@ -8323,10 +8323,10 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="C178" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="D178" t="s">
         <v>314</v>
@@ -8352,10 +8352,10 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="C179" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="D179" t="s">
         <v>314</v>
@@ -8382,10 +8382,10 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="C180" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="D180" t="s">
         <v>314</v>
@@ -8412,10 +8412,10 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="C181" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="D181" t="s">
         <v>314</v>
@@ -8441,10 +8441,10 @@
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="C182" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="D182" t="s">
         <v>314</v>
@@ -8470,10 +8470,10 @@
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="C183" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="D183" t="s">
         <v>314</v>
@@ -8500,10 +8500,10 @@
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C184" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D184" t="s">
         <v>314</v>
@@ -8530,10 +8530,10 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C185" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D185" t="s">
         <v>314</v>
@@ -8560,10 +8560,10 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C186" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="D186" t="s">
         <v>314</v>
@@ -8590,10 +8590,10 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="C187" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="D187" t="s">
         <v>314</v>
@@ -8620,10 +8620,10 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="C188" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="D188" t="s">
         <v>314</v>
@@ -8650,10 +8650,10 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="C189" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="D189" t="s">
         <v>314</v>
@@ -8680,10 +8680,10 @@
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C190" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="D190" t="s">
         <v>314</v>
@@ -8710,10 +8710,10 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="C191" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="D191" t="s">
         <v>314</v>
@@ -8739,10 +8739,10 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="C192" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="D192" t="s">
         <v>314</v>
@@ -8769,10 +8769,10 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="C193" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="D193" t="s">
         <v>314</v>
@@ -8799,10 +8799,10 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="C194" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="D194" t="s">
         <v>314</v>
@@ -8828,10 +8828,10 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="C195" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="D195" t="s">
         <v>314</v>
@@ -8858,10 +8858,10 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="C196" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="D196" t="s">
         <v>314</v>
@@ -8888,10 +8888,10 @@
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="C197" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="D197" t="s">
         <v>314</v>
@@ -8918,10 +8918,10 @@
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="C198" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="D198" t="s">
         <v>314</v>
@@ -8948,10 +8948,10 @@
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="C199" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="D199" t="s">
         <v>314</v>
@@ -8978,10 +8978,10 @@
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C200" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="D200" t="s">
         <v>314</v>
@@ -9007,10 +9007,10 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="C201" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="D201" t="s">
         <v>314</v>
@@ -9036,10 +9036,10 @@
         <v>201</v>
       </c>
       <c r="B202" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="C202" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="D202" t="s">
         <v>314</v>
@@ -9065,10 +9065,10 @@
         <v>202</v>
       </c>
       <c r="B203" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="C203" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="D203" t="s">
         <v>314</v>
@@ -9095,10 +9095,10 @@
         <v>203</v>
       </c>
       <c r="B204" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="C204" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="D204" t="s">
         <v>314</v>
@@ -9125,10 +9125,10 @@
         <v>204</v>
       </c>
       <c r="B205" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="C205" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="D205" t="s">
         <v>314</v>
@@ -9154,10 +9154,10 @@
         <v>205</v>
       </c>
       <c r="B206" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="C206" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="D206" t="s">
         <v>314</v>
@@ -9184,10 +9184,10 @@
         <v>206</v>
       </c>
       <c r="B207" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="C207" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="D207" t="s">
         <v>314</v>
@@ -9214,10 +9214,10 @@
         <v>207</v>
       </c>
       <c r="B208" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="C208" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="D208" t="s">
         <v>314</v>
@@ -9244,10 +9244,10 @@
         <v>208</v>
       </c>
       <c r="B209" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="C209" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="D209" t="s">
         <v>314</v>
@@ -9273,10 +9273,10 @@
         <v>209</v>
       </c>
       <c r="B210" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="C210" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="D210" t="s">
         <v>314</v>
@@ -9303,10 +9303,10 @@
         <v>210</v>
       </c>
       <c r="B211" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C211" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="D211" t="s">
         <v>314</v>
@@ -9333,10 +9333,10 @@
         <v>211</v>
       </c>
       <c r="B212" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="C212" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="D212" t="s">
         <v>314</v>
@@ -9363,10 +9363,10 @@
         <v>212</v>
       </c>
       <c r="B213" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="C213" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="D213" t="s">
         <v>314</v>
@@ -9393,10 +9393,10 @@
         <v>213</v>
       </c>
       <c r="B214" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="C214" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="D214" t="s">
         <v>314</v>
@@ -9423,10 +9423,10 @@
         <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="C215" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="D215" t="s">
         <v>314</v>
@@ -9453,10 +9453,10 @@
         <v>215</v>
       </c>
       <c r="B216" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="C216" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="D216" t="s">
         <v>314</v>
@@ -9483,10 +9483,10 @@
         <v>216</v>
       </c>
       <c r="B217" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="C217" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="D217" t="s">
         <v>314</v>
@@ -9513,10 +9513,10 @@
         <v>217</v>
       </c>
       <c r="B218" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="C218" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="D218" t="s">
         <v>314</v>
@@ -9543,10 +9543,10 @@
         <v>218</v>
       </c>
       <c r="B219" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="C219" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="D219" t="s">
         <v>314</v>
@@ -9573,10 +9573,10 @@
         <v>219</v>
       </c>
       <c r="B220" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="C220" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="D220" t="s">
         <v>314</v>
@@ -9602,10 +9602,10 @@
         <v>220</v>
       </c>
       <c r="B221" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="C221" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="D221" t="s">
         <v>314</v>
@@ -9632,10 +9632,10 @@
         <v>221</v>
       </c>
       <c r="B222" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="C222" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="D222" t="s">
         <v>314</v>
@@ -9662,10 +9662,10 @@
         <v>222</v>
       </c>
       <c r="B223" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="C223" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="D223" t="s">
         <v>314</v>
@@ -9692,10 +9692,10 @@
         <v>223</v>
       </c>
       <c r="B224" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="C224" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="D224" t="s">
         <v>314</v>
@@ -9721,10 +9721,10 @@
         <v>224</v>
       </c>
       <c r="B225" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="C225" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="D225" t="s">
         <v>314</v>
@@ -9750,10 +9750,10 @@
         <v>225</v>
       </c>
       <c r="B226" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="C226" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="D226" t="s">
         <v>314</v>
@@ -9779,10 +9779,10 @@
         <v>226</v>
       </c>
       <c r="B227" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="C227" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="D227" t="s">
         <v>314</v>
@@ -9809,10 +9809,10 @@
         <v>227</v>
       </c>
       <c r="B228" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="C228" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="D228" t="s">
         <v>314</v>
@@ -9839,10 +9839,10 @@
         <v>228</v>
       </c>
       <c r="B229" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="C229" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="D229" t="s">
         <v>314</v>
@@ -9868,10 +9868,10 @@
         <v>229</v>
       </c>
       <c r="B230" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="C230" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="D230" t="s">
         <v>314</v>
@@ -9898,10 +9898,10 @@
         <v>230</v>
       </c>
       <c r="B231" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="C231" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="D231" t="s">
         <v>314</v>
@@ -9928,10 +9928,10 @@
         <v>231</v>
       </c>
       <c r="B232" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="C232" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="D232" t="s">
         <v>314</v>
@@ -9958,10 +9958,10 @@
         <v>232</v>
       </c>
       <c r="B233" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="C233" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="D233" t="s">
         <v>314</v>
@@ -9988,10 +9988,10 @@
         <v>233</v>
       </c>
       <c r="B234" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="C234" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="D234" t="s">
         <v>314</v>
@@ -10018,10 +10018,10 @@
         <v>234</v>
       </c>
       <c r="B235" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="C235" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="D235" t="s">
         <v>314</v>
@@ -10048,10 +10048,10 @@
         <v>235</v>
       </c>
       <c r="B236" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="C236" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D236" t="s">
         <v>314</v>
@@ -10078,10 +10078,10 @@
         <v>236</v>
       </c>
       <c r="B237" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C237" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="D237" t="s">
         <v>314</v>
@@ -10107,10 +10107,10 @@
         <v>237</v>
       </c>
       <c r="B238" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="C238" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="D238" t="s">
         <v>314</v>
@@ -10136,10 +10136,10 @@
         <v>238</v>
       </c>
       <c r="B239" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="C239" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="D239" t="s">
         <v>314</v>
@@ -10166,10 +10166,10 @@
         <v>239</v>
       </c>
       <c r="B240" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="C240" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="D240" t="s">
         <v>314</v>
@@ -10196,10 +10196,10 @@
         <v>240</v>
       </c>
       <c r="B241" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="C241" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="D241" t="s">
         <v>314</v>
@@ -10226,10 +10226,10 @@
         <v>241</v>
       </c>
       <c r="B242" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="C242" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="D242" t="s">
         <v>314</v>
@@ -10256,10 +10256,10 @@
         <v>242</v>
       </c>
       <c r="B243" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="C243" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="D243" t="s">
         <v>314</v>
@@ -10285,10 +10285,10 @@
         <v>243</v>
       </c>
       <c r="B244" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="C244" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="D244" t="s">
         <v>314</v>
@@ -10314,10 +10314,10 @@
         <v>244</v>
       </c>
       <c r="B245" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="C245" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="D245" t="s">
         <v>314</v>
@@ -10344,10 +10344,10 @@
         <v>245</v>
       </c>
       <c r="B246" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="C246" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="D246" t="s">
         <v>314</v>
@@ -10374,10 +10374,10 @@
         <v>246</v>
       </c>
       <c r="B247" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="C247" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="D247" t="s">
         <v>314</v>
@@ -10404,10 +10404,10 @@
         <v>247</v>
       </c>
       <c r="B248" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="C248" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="D248" t="s">
         <v>314</v>
@@ -10434,10 +10434,10 @@
         <v>248</v>
       </c>
       <c r="B249" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="C249" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="D249" t="s">
         <v>314</v>
@@ -10464,10 +10464,10 @@
         <v>249</v>
       </c>
       <c r="B250" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="C250" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="D250" t="s">
         <v>314</v>
@@ -10494,10 +10494,10 @@
         <v>250</v>
       </c>
       <c r="B251" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="C251" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="D251" t="s">
         <v>314</v>
@@ -10524,10 +10524,10 @@
         <v>251</v>
       </c>
       <c r="B252" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="C252" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="D252" t="s">
         <v>314</v>
@@ -10554,10 +10554,10 @@
         <v>252</v>
       </c>
       <c r="B253" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="C253" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="D253" t="s">
         <v>314</v>
@@ -10584,10 +10584,10 @@
         <v>253</v>
       </c>
       <c r="B254" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="C254" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="D254" t="s">
         <v>314</v>
@@ -10614,10 +10614,10 @@
         <v>254</v>
       </c>
       <c r="B255" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="C255" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="D255" t="s">
         <v>314</v>
@@ -10643,10 +10643,10 @@
         <v>255</v>
       </c>
       <c r="B256" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="C256" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="D256" t="s">
         <v>314</v>
@@ -10673,10 +10673,10 @@
         <v>256</v>
       </c>
       <c r="B257" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C257" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="D257" t="s">
         <v>314</v>
@@ -10702,10 +10702,10 @@
         <v>257</v>
       </c>
       <c r="B258" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="C258" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="D258" t="s">
         <v>314</v>
@@ -10731,10 +10731,10 @@
         <v>258</v>
       </c>
       <c r="B259" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="C259" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="D259" t="s">
         <v>314</v>
@@ -10760,10 +10760,10 @@
         <v>259</v>
       </c>
       <c r="B260" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="C260" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="D260" t="s">
         <v>314</v>
@@ -10790,10 +10790,10 @@
         <v>260</v>
       </c>
       <c r="B261" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="C261" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="D261" t="s">
         <v>314</v>
@@ -10820,10 +10820,10 @@
         <v>261</v>
       </c>
       <c r="B262" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="C262" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="D262" t="s">
         <v>314</v>
@@ -10850,10 +10850,10 @@
         <v>262</v>
       </c>
       <c r="B263" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="C263" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="D263" t="s">
         <v>314</v>
@@ -10880,10 +10880,10 @@
         <v>263</v>
       </c>
       <c r="B264" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="C264" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="D264" t="s">
         <v>314</v>
@@ -10910,10 +10910,10 @@
         <v>264</v>
       </c>
       <c r="B265" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="C265" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="D265" t="s">
         <v>314</v>
@@ -10939,10 +10939,10 @@
         <v>265</v>
       </c>
       <c r="B266" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="C266" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="D266" t="s">
         <v>314</v>
@@ -10968,10 +10968,10 @@
         <v>266</v>
       </c>
       <c r="B267" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="C267" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="D267" t="s">
         <v>314</v>
@@ -10998,10 +10998,10 @@
         <v>267</v>
       </c>
       <c r="B268" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="C268" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="D268" t="s">
         <v>314</v>
@@ -11028,10 +11028,10 @@
         <v>268</v>
       </c>
       <c r="B269" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="C269" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="D269" t="s">
         <v>314</v>
@@ -11058,10 +11058,10 @@
         <v>269</v>
       </c>
       <c r="B270" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="C270" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="D270" t="s">
         <v>314</v>
@@ -11087,10 +11087,10 @@
         <v>270</v>
       </c>
       <c r="B271" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="C271" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="D271" t="s">
         <v>314</v>
@@ -11117,10 +11117,10 @@
         <v>271</v>
       </c>
       <c r="B272" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="C272" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="D272" t="s">
         <v>314</v>
@@ -11146,10 +11146,10 @@
         <v>272</v>
       </c>
       <c r="B273" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="C273" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="D273" t="s">
         <v>314</v>
@@ -11176,10 +11176,10 @@
         <v>273</v>
       </c>
       <c r="B274" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="C274" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="D274" t="s">
         <v>314</v>
@@ -11205,10 +11205,10 @@
         <v>274</v>
       </c>
       <c r="B275" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="C275" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="D275" t="s">
         <v>314</v>
@@ -11235,10 +11235,10 @@
         <v>275</v>
       </c>
       <c r="B276" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="C276" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="D276" t="s">
         <v>314</v>
@@ -11265,10 +11265,10 @@
         <v>276</v>
       </c>
       <c r="B277" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="C277" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="D277" t="s">
         <v>314</v>
@@ -11295,10 +11295,10 @@
         <v>277</v>
       </c>
       <c r="B278" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="C278" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="D278" t="s">
         <v>314</v>
@@ -11324,10 +11324,10 @@
         <v>278</v>
       </c>
       <c r="B279" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="C279" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="D279" t="s">
         <v>314</v>
@@ -11354,10 +11354,10 @@
         <v>279</v>
       </c>
       <c r="B280" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="C280" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="D280" t="s">
         <v>314</v>
@@ -11384,10 +11384,10 @@
         <v>280</v>
       </c>
       <c r="B281" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="C281" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="D281" t="s">
         <v>314</v>
@@ -11414,10 +11414,10 @@
         <v>281</v>
       </c>
       <c r="B282" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="C282" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="D282" t="s">
         <v>314</v>
@@ -11443,10 +11443,10 @@
         <v>282</v>
       </c>
       <c r="B283" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="C283" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="D283" t="s">
         <v>314</v>
@@ -11473,10 +11473,10 @@
         <v>283</v>
       </c>
       <c r="B284" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="C284" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="D284" t="s">
         <v>314</v>
@@ -11503,10 +11503,10 @@
         <v>284</v>
       </c>
       <c r="B285" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="C285" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="D285" t="s">
         <v>314</v>
@@ -11533,10 +11533,10 @@
         <v>285</v>
       </c>
       <c r="B286" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="C286" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="D286" t="s">
         <v>314</v>
@@ -11563,10 +11563,10 @@
         <v>286</v>
       </c>
       <c r="B287" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="C287" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="D287" t="s">
         <v>314</v>
@@ -11592,10 +11592,10 @@
         <v>287</v>
       </c>
       <c r="B288" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="C288" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="D288" t="s">
         <v>314</v>
@@ -11621,10 +11621,10 @@
         <v>288</v>
       </c>
       <c r="B289" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="C289" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="D289" t="s">
         <v>314</v>
@@ -11651,10 +11651,10 @@
         <v>289</v>
       </c>
       <c r="B290" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="C290" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="D290" t="s">
         <v>314</v>
@@ -11681,10 +11681,10 @@
         <v>290</v>
       </c>
       <c r="B291" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="C291" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="D291" t="s">
         <v>314</v>
@@ -11711,10 +11711,10 @@
         <v>291</v>
       </c>
       <c r="B292" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="C292" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="D292" t="s">
         <v>314</v>
@@ -11741,10 +11741,10 @@
         <v>292</v>
       </c>
       <c r="B293" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="C293" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="D293" t="s">
         <v>314</v>
@@ -11771,10 +11771,10 @@
         <v>293</v>
       </c>
       <c r="B294" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="C294" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="D294" t="s">
         <v>314</v>
@@ -11801,10 +11801,10 @@
         <v>294</v>
       </c>
       <c r="B295" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="C295" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="D295" t="s">
         <v>314</v>
@@ -11831,10 +11831,10 @@
         <v>295</v>
       </c>
       <c r="B296" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="C296" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="D296" t="s">
         <v>314</v>
@@ -11861,10 +11861,10 @@
         <v>296</v>
       </c>
       <c r="B297" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="C297" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="D297" t="s">
         <v>314</v>
@@ -11890,10 +11890,10 @@
         <v>297</v>
       </c>
       <c r="B298" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="C298" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="D298" t="s">
         <v>314</v>
@@ -11919,10 +11919,10 @@
         <v>298</v>
       </c>
       <c r="B299" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="C299" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="D299" t="s">
         <v>314</v>
@@ -11949,10 +11949,10 @@
         <v>299</v>
       </c>
       <c r="B300" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="C300" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="D300" t="s">
         <v>314</v>
@@ -11978,10 +11978,10 @@
         <v>300</v>
       </c>
       <c r="B301" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="C301" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="D301" t="s">
         <v>314</v>
@@ -12008,10 +12008,10 @@
         <v>301</v>
       </c>
       <c r="B302" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="C302" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="D302" t="s">
         <v>314</v>
@@ -12038,10 +12038,10 @@
         <v>302</v>
       </c>
       <c r="B303" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="C303" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="D303" t="s">
         <v>314</v>
@@ -12067,10 +12067,10 @@
         <v>303</v>
       </c>
       <c r="B304" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="C304" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="D304" t="s">
         <v>314</v>
@@ -12096,10 +12096,10 @@
         <v>304</v>
       </c>
       <c r="B305" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="C305" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="D305" t="s">
         <v>314</v>
@@ -12126,10 +12126,10 @@
         <v>305</v>
       </c>
       <c r="B306" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="C306" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="D306" t="s">
         <v>314</v>
@@ -12155,10 +12155,10 @@
         <v>306</v>
       </c>
       <c r="B307" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="C307" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="D307" t="s">
         <v>314</v>
@@ -12185,10 +12185,10 @@
         <v>307</v>
       </c>
       <c r="B308" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="C308" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="D308" t="s">
         <v>314</v>
@@ -12215,10 +12215,10 @@
         <v>308</v>
       </c>
       <c r="B309" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="C309" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="D309" t="s">
         <v>314</v>
@@ -12244,10 +12244,10 @@
         <v>309</v>
       </c>
       <c r="B310" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="C310" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="D310" t="s">
         <v>314</v>
@@ -12273,10 +12273,10 @@
         <v>310</v>
       </c>
       <c r="B311" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="C311" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="D311" t="s">
         <v>314</v>
@@ -12303,10 +12303,10 @@
         <v>311</v>
       </c>
       <c r="B312" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="C312" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="D312" t="s">
         <v>314</v>
@@ -12332,10 +12332,10 @@
         <v>312</v>
       </c>
       <c r="B313" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="C313" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="D313" t="s">
         <v>314</v>
@@ -12362,10 +12362,10 @@
         <v>313</v>
       </c>
       <c r="B314" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="C314" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="D314" t="s">
         <v>314</v>
@@ -12391,10 +12391,10 @@
         <v>314</v>
       </c>
       <c r="B315" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="C315" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="D315" t="s">
         <v>314</v>
@@ -12420,10 +12420,10 @@
         <v>315</v>
       </c>
       <c r="B316" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="C316" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="D316" t="s">
         <v>314</v>
@@ -12450,10 +12450,10 @@
         <v>316</v>
       </c>
       <c r="B317" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="C317" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="D317" t="s">
         <v>314</v>
@@ -12479,10 +12479,10 @@
         <v>317</v>
       </c>
       <c r="B318" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="C318" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="D318" t="s">
         <v>314</v>
@@ -12509,10 +12509,10 @@
         <v>318</v>
       </c>
       <c r="B319" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="C319" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="D319" t="s">
         <v>314</v>
@@ -12538,10 +12538,10 @@
         <v>319</v>
       </c>
       <c r="B320" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="C320" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="D320" t="s">
         <v>314</v>
@@ -12568,10 +12568,10 @@
         <v>320</v>
       </c>
       <c r="B321" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="C321" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="D321" t="s">
         <v>314</v>
@@ -12597,10 +12597,10 @@
         <v>321</v>
       </c>
       <c r="B322" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="C322" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="D322" t="s">
         <v>314</v>
@@ -12627,10 +12627,10 @@
         <v>322</v>
       </c>
       <c r="B323" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="C323" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="D323" t="s">
         <v>314</v>
@@ -12657,10 +12657,10 @@
         <v>323</v>
       </c>
       <c r="B324" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="C324" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="D324" t="s">
         <v>314</v>
@@ -12686,10 +12686,10 @@
         <v>324</v>
       </c>
       <c r="B325" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="C325" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="D325" t="s">
         <v>314</v>
@@ -12716,10 +12716,10 @@
         <v>325</v>
       </c>
       <c r="B326" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="C326" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="D326" t="s">
         <v>314</v>
@@ -12746,10 +12746,10 @@
         <v>326</v>
       </c>
       <c r="B327" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="C327" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="D327" t="s">
         <v>314</v>
@@ -12776,10 +12776,10 @@
         <v>327</v>
       </c>
       <c r="B328" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="C328" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="D328" t="s">
         <v>314</v>
@@ -12805,10 +12805,10 @@
         <v>328</v>
       </c>
       <c r="B329" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="C329" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="D329" t="s">
         <v>314</v>
@@ -12835,10 +12835,10 @@
         <v>329</v>
       </c>
       <c r="B330" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="C330" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="D330" t="s">
         <v>314</v>
@@ -12865,10 +12865,10 @@
         <v>330</v>
       </c>
       <c r="B331" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="C331" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="D331" t="s">
         <v>314</v>
@@ -12895,10 +12895,10 @@
         <v>331</v>
       </c>
       <c r="B332" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="C332" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="D332" t="s">
         <v>314</v>
@@ -12924,10 +12924,10 @@
         <v>332</v>
       </c>
       <c r="B333" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="C333" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="D333" t="s">
         <v>314</v>
@@ -12953,10 +12953,10 @@
         <v>333</v>
       </c>
       <c r="B334" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="C334" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="D334" t="s">
         <v>314</v>
@@ -12983,10 +12983,10 @@
         <v>334</v>
       </c>
       <c r="B335" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="C335" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="D335" t="s">
         <v>314</v>
@@ -13013,10 +13013,10 @@
         <v>335</v>
       </c>
       <c r="B336" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="C336" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="D336" t="s">
         <v>314</v>
@@ -13043,10 +13043,10 @@
         <v>336</v>
       </c>
       <c r="B337" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="C337" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="D337" t="s">
         <v>314</v>
@@ -13073,10 +13073,10 @@
         <v>337</v>
       </c>
       <c r="B338" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="C338" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="D338" t="s">
         <v>314</v>
@@ -13103,10 +13103,10 @@
         <v>338</v>
       </c>
       <c r="B339" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="C339" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="D339" t="s">
         <v>314</v>
@@ -13133,10 +13133,10 @@
         <v>339</v>
       </c>
       <c r="B340" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="C340" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="D340" t="s">
         <v>314</v>
@@ -13163,10 +13163,10 @@
         <v>340</v>
       </c>
       <c r="B341" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="C341" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="D341" t="s">
         <v>314</v>
@@ -13192,10 +13192,10 @@
         <v>341</v>
       </c>
       <c r="B342" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="C342" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="D342" t="s">
         <v>314</v>
@@ -13222,10 +13222,10 @@
         <v>342</v>
       </c>
       <c r="B343" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="C343" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="D343" t="s">
         <v>314</v>
@@ -13252,10 +13252,10 @@
         <v>343</v>
       </c>
       <c r="B344" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="C344" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="D344" t="s">
         <v>314</v>
@@ -13281,10 +13281,10 @@
         <v>344</v>
       </c>
       <c r="B345" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="C345" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="D345" t="s">
         <v>314</v>
@@ -13311,10 +13311,10 @@
         <v>345</v>
       </c>
       <c r="B346" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="C346" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="D346" t="s">
         <v>314</v>
@@ -13341,10 +13341,10 @@
         <v>346</v>
       </c>
       <c r="B347" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="C347" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="D347" t="s">
         <v>314</v>
@@ -13454,7 +13454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3414857B-17AF-4107-83E0-9CC76FB79584}">
   <dimension ref="A1:F725"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+    <sheetView topLeftCell="A172" workbookViewId="0">
       <selection activeCell="D183" sqref="D183"/>
     </sheetView>
   </sheetViews>
@@ -19531,7 +19531,7 @@
         <v>1</v>
       </c>
       <c r="E544" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="545" spans="1:5" x14ac:dyDescent="0.3">
@@ -19561,7 +19561,7 @@
         <v>1</v>
       </c>
       <c r="E546" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="547" spans="1:5" x14ac:dyDescent="0.3">
@@ -19576,7 +19576,7 @@
         <v>1</v>
       </c>
       <c r="E547" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
     </row>
     <row r="548" spans="1:5" x14ac:dyDescent="0.3">
@@ -19621,7 +19621,7 @@
         <v>1</v>
       </c>
       <c r="E550" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
     </row>
     <row r="551" spans="1:5" x14ac:dyDescent="0.3">
@@ -19741,7 +19741,7 @@
         <v>1</v>
       </c>
       <c r="E558" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
     </row>
     <row r="559" spans="1:5" x14ac:dyDescent="0.3">
@@ -19756,7 +19756,7 @@
         <v>3</v>
       </c>
       <c r="E559" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
     </row>
     <row r="560" spans="1:5" x14ac:dyDescent="0.3">
@@ -19771,7 +19771,7 @@
         <v>1</v>
       </c>
       <c r="E560" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="561" spans="1:5" x14ac:dyDescent="0.3">
@@ -20056,7 +20056,7 @@
         <v>1</v>
       </c>
       <c r="E579" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
     </row>
     <row r="580" spans="1:5" x14ac:dyDescent="0.3">
@@ -20341,7 +20341,7 @@
         <v>1</v>
       </c>
       <c r="E598" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="599" spans="1:5" x14ac:dyDescent="0.3">
@@ -20356,7 +20356,7 @@
         <v>1</v>
       </c>
       <c r="E599" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="600" spans="1:5" x14ac:dyDescent="0.3">
@@ -20386,7 +20386,7 @@
         <v>1</v>
       </c>
       <c r="E601" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
     </row>
     <row r="602" spans="1:5" x14ac:dyDescent="0.3">
@@ -20461,7 +20461,7 @@
         <v>1</v>
       </c>
       <c r="E606" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="607" spans="1:5" x14ac:dyDescent="0.3">
@@ -20521,7 +20521,7 @@
         <v>1</v>
       </c>
       <c r="E610" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="611" spans="1:5" x14ac:dyDescent="0.3">
@@ -20656,7 +20656,7 @@
         <v>1</v>
       </c>
       <c r="E619" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="620" spans="1:5" x14ac:dyDescent="0.3">
@@ -20701,7 +20701,7 @@
         <v>1</v>
       </c>
       <c r="E622" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="623" spans="1:5" x14ac:dyDescent="0.3">
@@ -20941,7 +20941,7 @@
         <v>1</v>
       </c>
       <c r="E638" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
     </row>
     <row r="639" spans="1:5" x14ac:dyDescent="0.3">
@@ -20956,7 +20956,7 @@
         <v>1</v>
       </c>
       <c r="E639" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="640" spans="1:5" x14ac:dyDescent="0.3">
@@ -21091,7 +21091,7 @@
         <v>1</v>
       </c>
       <c r="E648" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="649" spans="1:5" x14ac:dyDescent="0.3">
@@ -21241,7 +21241,7 @@
         <v>1</v>
       </c>
       <c r="E658" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="659" spans="1:5" x14ac:dyDescent="0.3">
@@ -21526,7 +21526,7 @@
         <v>1</v>
       </c>
       <c r="E677" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="678" spans="1:5" x14ac:dyDescent="0.3">
@@ -21541,7 +21541,7 @@
         <v>2</v>
       </c>
       <c r="E678" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="679" spans="1:5" x14ac:dyDescent="0.3">
@@ -21706,7 +21706,7 @@
         <v>1</v>
       </c>
       <c r="E689" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="690" spans="1:5" x14ac:dyDescent="0.3">
@@ -21736,7 +21736,7 @@
         <v>1</v>
       </c>
       <c r="E691" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="692" spans="1:5" x14ac:dyDescent="0.3">
@@ -21931,7 +21931,7 @@
         <v>1</v>
       </c>
       <c r="E704" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="705" spans="1:5" x14ac:dyDescent="0.3">
@@ -21961,7 +21961,7 @@
         <v>3</v>
       </c>
       <c r="E706" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
     </row>
     <row r="707" spans="1:5" x14ac:dyDescent="0.3">
@@ -22036,7 +22036,7 @@
         <v>1</v>
       </c>
       <c r="E711" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="712" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>